<commit_message>
Completed I2C Driver (untested)
</commit_message>
<xml_diff>
--- a/Hardware/Design/Main Board/bom/amp_bom_only.xlsx
+++ b/Hardware/Design/Main Board/bom/amp_bom_only.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/69f5ad8fb782b24f/Documents/Power Amp/Manufacturing Files/amp board/bom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/69f5ad8fb782b24f/Documents/GitHub/Home-Audio-System/Hardware/Design/Main Board/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{04327A53-7620-40AA-B0F5-66EFCFAEF841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{425CF121-2A4F-4AB3-9D48-A6C236A3FBDD}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{04327A53-7620-40AA-B0F5-66EFCFAEF841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EBC9407-8628-44EB-855B-ED2C4B4A9383}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{EC4EE303-9F8E-478B-9455-4E26A4F347FC}"/>
+    <workbookView xWindow="3345" yWindow="4215" windowWidth="28800" windowHeight="15345" xr2:uid="{EC4EE303-9F8E-478B-9455-4E26A4F347FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1850,10 +1850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A842EA08-1615-483D-83DC-F58A051786BC}">
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="K232" sqref="K232"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="J145" sqref="J145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5062,6 +5062,12 @@
         <v>1</v>
       </c>
     </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I154">
+        <f>SUM(I2:I152)</f>
+        <v>682</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>